<commit_message>
Fixed bug with auth retries
</commit_message>
<xml_diff>
--- a/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDP Network Map V2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Pycharm Projects\CDP_Network_Audit\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959F03D2-C9F0-4F6A-808F-30F127FB5943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2823B8-0B3D-433E-9DF9-B3E7B62DE94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
@@ -273,7 +273,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -613,60 +624,60 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="50.6640625" customWidth="1"/>
-    <col min="8" max="8" width="120.6640625" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="1" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="8" max="8" width="120.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -711,27 +722,27 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="19"/>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="20"/>
     </row>
-    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -745,6 +756,11 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DNS Resolution Failed">
+      <formula>NOT(ISERROR(SEARCH("DNS Resolution Failed",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -757,23 +773,23 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="21"/>
     </row>
-    <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
     </row>
-    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -794,23 +810,23 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="23"/>
     </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
     </row>
-    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Change to conditional formatting
</commit_message>
<xml_diff>
--- a/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Pycharm Projects\CDP_Network_Audit\config_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDP Network Audit\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2823B8-0B3D-433E-9DF9-B3E7B62DE94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BF2788-304D-46B1-9D81-A89A7F088853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
     <t>Connection Errors</t>
   </si>
   <si>
-    <t>DNS Resolved IP Addresses</t>
+    <t>Reverse DNS Lookup</t>
   </si>
 </sst>
 </file>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -246,12 +246,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -268,6 +262,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,7 +618,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,14 +729,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
-      <c r="B2" s="20"/>
+      <c r="B2" s="18"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -779,14 +776,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -816,14 +813,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reduced size of code and added collecion of serial numbers and uptime information
</commit_message>
<xml_diff>
--- a/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDP Network Audit\config_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://muellergroup-my.sharepoint.com/personal/christopher_davies1_muller_co_uk/Documents/Documents/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BF2788-304D-46B1-9D81-A89A7F088853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_D2F56CADE1FA449E3C00BDB9D3946FD25E83B71C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B015EDC1-1FFB-48B0-B182-7126EB43D8D6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
@@ -19,19 +19,22 @@
     <sheet name="Authentication Errors" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Audit!$A$11:$I$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Audit!$A$11:$K$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNS Resolved'!$A$4:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>CDP Device Audit</t>
   </si>
   <si>
+    <t>Site Code:</t>
+  </si>
+  <si>
     <t>Date:</t>
   </si>
   <si>
@@ -41,12 +44,12 @@
     <t>Seed Device 1:</t>
   </si>
   <si>
+    <t>10.145.63.1</t>
+  </si>
+  <si>
     <t>Seed Device 2:</t>
   </si>
   <si>
-    <t>Site Code:</t>
-  </si>
-  <si>
     <t>LOCAL_HOST</t>
   </si>
   <si>
@@ -74,19 +77,61 @@
     <t>CAPABILITIES</t>
   </si>
   <si>
+    <t>GB-CAY2-001CSW001</t>
+  </si>
+  <si>
+    <t>GB-CAY2-001ASW001</t>
+  </si>
+  <si>
+    <t>10.145.61.10</t>
+  </si>
+  <si>
+    <t>10.250.16.17</t>
+  </si>
+  <si>
+    <t>10.250.16.21</t>
+  </si>
+  <si>
+    <t>gb-cay2-001sdw101</t>
+  </si>
+  <si>
+    <t>62.172.66.138</t>
+  </si>
+  <si>
+    <t>10.250.16.18</t>
+  </si>
+  <si>
+    <t>gb-cay2-001sdw102</t>
+  </si>
+  <si>
+    <t>10.250.16.22</t>
+  </si>
+  <si>
+    <t>Reverse DNS Lookup</t>
+  </si>
+  <si>
+    <t>Hostname</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>10.255.145.61</t>
+  </si>
+  <si>
+    <t>10.255.145.62</t>
+  </si>
+  <si>
+    <t>Connection Errors</t>
+  </si>
+  <si>
     <t>Authentication Errors</t>
   </si>
   <si>
-    <t>Hostname</t>
-  </si>
-  <si>
-    <t>IP Address</t>
-  </si>
-  <si>
-    <t>Connection Errors</t>
-  </si>
-  <si>
-    <t>Reverse DNS Lookup</t>
+    <t>UPTIME</t>
+  </si>
+  <si>
+    <t>Serial</t>
   </si>
 </sst>
 </file>
@@ -150,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -191,11 +236,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -233,38 +289,28 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,143 +661,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
-    <col min="8" max="8" width="120.7109375" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="1" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="50.6640625" customWidth="1"/>
+    <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="108.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="K11" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A11:I11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A11:I11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="2">
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF264A58-7302-43F4-8536-3DC3756319EC}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>17</v>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:B4" xr:uid="{CF264A58-7302-43F4-8536-3DC3756319EC}"/>
+  <autoFilter ref="A4:B4" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="2">
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DNS Resolution Failed">
@@ -763,32 +849,52 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BC569B-A16A-4198-9DB5-FADCB4818C57}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>18</v>
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="B1" s="19"/>
     </row>
-    <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -800,32 +906,37 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1C2847-EC79-480E-B4B3-31C0E0F06CAB}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="21"/>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reduced size of code and added collection of serial numbers and uptime information
</commit_message>
<xml_diff>
--- a/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://muellergroup-my.sharepoint.com/personal/christopher_davies1_muller_co_uk/Documents/Documents/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Pycharm Projects\CDP_Network_Audit\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_D2F56CADE1FA449E3C00BDB9D3946FD25E83B71C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B015EDC1-1FFB-48B0-B182-7126EB43D8D6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330638E0-A6FC-4D22-99E4-799FD8C98595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
@@ -128,10 +128,10 @@
     <t>Authentication Errors</t>
   </si>
   <si>
-    <t>UPTIME</t>
-  </si>
-  <si>
-    <t>Serial</t>
+    <t>LOCAL UPTIME</t>
+  </si>
+  <si>
+    <t>LOCAL SERIAL</t>
   </si>
 </sst>
 </file>
@@ -251,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -289,6 +289,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -309,8 +312,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,65 +670,81 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="50.6640625" customWidth="1"/>
-    <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="108.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="108.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -732,20 +754,20 @@
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>33</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>13</v>
@@ -759,9 +781,17 @@
     </row>
   </sheetData>
   <autoFilter ref="A11:I11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="2">
+  <mergeCells count="10">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -776,24 +806,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="16"/>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -801,7 +831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -809,7 +839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -817,7 +847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -825,7 +855,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -856,43 +886,43 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="19"/>
-    </row>
-    <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -913,28 +943,28 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="19"/>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>

</xml_diff>